<commit_message>
update bpsk demodulator to include pulse filter before slicer
</commit_message>
<xml_diff>
--- a/LoopIntegralReference.xlsx
+++ b/LoopIntegralReference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninocarrillo/github/N9600A-sim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E419CA87-4147-794B-B428-A9EF63C7087C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FED85A-C235-FF41-BBE2-809C609B5EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="40" windowWidth="28760" windowHeight="14380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -419,7 +419,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -500,6 +500,9 @@
         <f>ROUND((F4+F4*G4) * $B$1/($B$2*D4*B4),0)</f>
         <v>2370370</v>
       </c>
+      <c r="I4">
+        <v>0.87</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -520,14 +523,14 @@
         <v>6554</v>
       </c>
       <c r="F5">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="G5" s="1">
         <v>0.5</v>
       </c>
       <c r="H5">
         <f t="shared" ref="H5:H7" si="1">ROUND((F5+F5*G5) * $B$1/($B$2*D5*B5),0)</f>
-        <v>742029</v>
+        <v>371014</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -557,6 +560,9 @@
       <c r="H6">
         <f t="shared" si="1"/>
         <v>824477</v>
+      </c>
+      <c r="I6">
+        <v>0.87</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
improve gfsk 9600 filter
</commit_message>
<xml_diff>
--- a/LoopIntegralReference.xlsx
+++ b/LoopIntegralReference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninocarrillo/github/N9600A-sim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA14B3BE-7E62-684C-9977-FE7646672B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0627B202-FA3D-B04C-B52D-FEE124373629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="40" windowWidth="28760" windowHeight="14380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -419,7 +419,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
qpsk 600 retune 1
</commit_message>
<xml_diff>
--- a/LoopIntegralReference.xlsx
+++ b/LoopIntegralReference.xlsx
@@ -547,7 +547,7 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1107,7 +1107,7 @@
         <v>0.5</v>
       </c>
       <c r="H36" s="12">
-        <f>ROUND(((F36*(1+G36)) * $B$26/$B$27)/B36, 0)</f>
+        <f>ROUND(((F36*(1+G36)) * $B$32/$B$33)/B36, 0)</f>
         <v>9481481</v>
       </c>
       <c r="I36" s="12">
@@ -1214,7 +1214,7 @@
         <v>0.5</v>
       </c>
       <c r="H42" s="12">
-        <f>ROUND(((F42*(1+G42)) * $B$26/$B$27)/B42, 0)</f>
+        <f>ROUND(((F42*(1+G42)) * $B$38/$B$39)/B42, 0)</f>
         <v>853333</v>
       </c>
       <c r="I42" s="12">

</xml_diff>

<commit_message>
qpsk 600 good retune
</commit_message>
<xml_diff>
--- a/LoopIntegralReference.xlsx
+++ b/LoopIntegralReference.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninocarrillo/github/N9600A-sim/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE3066C-0EBD-574F-9858-80AE6666E3C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="40" windowWidth="16780" windowHeight="14380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11985" yWindow="45" windowWidth="16785" windowHeight="14385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -91,8 +85,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,9 +248,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -294,7 +288,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -328,7 +322,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -363,10 +356,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -539,27 +531,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1">
       <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
@@ -573,7 +565,7 @@
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -589,7 +581,7 @@
       <c r="I2" s="4"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -605,7 +597,7 @@
       <c r="I3" s="7"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" s="6"/>
       <c r="B4" t="s">
         <v>8</v>
@@ -623,7 +615,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" s="6"/>
       <c r="B5" t="s">
         <v>4</v>
@@ -633,7 +625,7 @@
       </c>
       <c r="J5" s="9"/>
     </row>
-    <row r="6" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15.75" thickBot="1">
       <c r="A6" s="10" t="s">
         <v>0</v>
       </c>
@@ -669,8 +661,8 @@
         <v>28.414244433257871</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="15.75" thickBot="1"/>
+    <row r="8" spans="1:12">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -686,7 +678,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
@@ -702,7 +694,7 @@
       <c r="I9" s="7"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10" s="6"/>
       <c r="B10" t="s">
         <v>8</v>
@@ -720,7 +712,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="A11" s="6"/>
       <c r="B11" t="s">
         <v>4</v>
@@ -730,7 +722,7 @@
       </c>
       <c r="J11" s="9"/>
     </row>
-    <row r="12" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15.75" thickBot="1">
       <c r="A12" s="10" t="s">
         <v>2</v>
       </c>
@@ -766,10 +758,10 @@
         <v>28.414244433257871</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="15.75" thickBot="1">
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
@@ -785,7 +777,7 @@
       <c r="I14" s="4"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="A15" s="6" t="s">
         <v>6</v>
       </c>
@@ -804,7 +796,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="A16" s="6"/>
       <c r="B16" t="s">
         <v>8</v>
@@ -822,7 +814,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12">
       <c r="A17" s="6"/>
       <c r="B17" t="s">
         <v>4</v>
@@ -832,7 +824,7 @@
       </c>
       <c r="J17" s="9"/>
     </row>
-    <row r="18" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="15.75" thickBot="1">
       <c r="A18" s="10" t="s">
         <v>1</v>
       </c>
@@ -868,8 +860,8 @@
         <v>27.424608507342434</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="15.75" thickBot="1"/>
+    <row r="20" spans="1:12">
       <c r="A20" s="2" t="s">
         <v>5</v>
       </c>
@@ -885,7 +877,7 @@
       <c r="I20" s="4"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="A21" s="6" t="s">
         <v>6</v>
       </c>
@@ -904,7 +896,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12">
       <c r="A22" s="6"/>
       <c r="B22" t="s">
         <v>8</v>
@@ -922,7 +914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12">
       <c r="A23" s="6"/>
       <c r="B23" t="s">
         <v>4</v>
@@ -932,7 +924,7 @@
       </c>
       <c r="J23" s="9"/>
     </row>
-    <row r="24" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="15.75" thickBot="1">
       <c r="A24" s="10" t="s">
         <v>1</v>
       </c>
@@ -968,8 +960,8 @@
         <v>27.659196283614612</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="15.75" thickBot="1"/>
+    <row r="26" spans="1:12">
       <c r="A26" s="2" t="s">
         <v>5</v>
       </c>
@@ -985,7 +977,7 @@
       <c r="I26" s="4"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12">
       <c r="A27" s="6" t="s">
         <v>6</v>
       </c>
@@ -1001,7 +993,7 @@
       <c r="I27" s="7"/>
       <c r="J27" s="8"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12">
       <c r="A28" s="6"/>
       <c r="B28" t="s">
         <v>8</v>
@@ -1022,7 +1014,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12">
       <c r="A29" s="6"/>
       <c r="B29" t="s">
         <v>4</v>
@@ -1035,7 +1027,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="15.75" thickBot="1">
       <c r="A30" s="10" t="s">
         <v>3</v>
       </c>
@@ -1071,8 +1063,8 @@
         <v>28.416995678270762</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="15.75" thickBot="1"/>
+    <row r="32" spans="1:12">
       <c r="A32" s="2" t="s">
         <v>5</v>
       </c>
@@ -1088,7 +1080,7 @@
       <c r="I32" s="4"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12">
       <c r="A33" s="6" t="s">
         <v>6</v>
       </c>
@@ -1104,7 +1096,7 @@
       <c r="I33" s="7"/>
       <c r="J33" s="8"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12">
       <c r="A34" s="6"/>
       <c r="B34" t="s">
         <v>8</v>
@@ -1125,7 +1117,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12">
       <c r="A35" s="6"/>
       <c r="B35" t="s">
         <v>4</v>
@@ -1138,7 +1130,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="15.75" thickBot="1">
       <c r="A36" s="10" t="s">
         <v>3</v>
       </c>
@@ -1184,24 +1176,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
reduce qpsk 600 offset
</commit_message>
<xml_diff>
--- a/LoopIntegralReference.xlsx
+++ b/LoopIntegralReference.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="20">
   <si>
     <t>BPSK 300</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>adjust for 25 hz offset</t>
+  </si>
+  <si>
+    <t>adjust for 13 hz offset</t>
   </si>
 </sst>
 </file>
@@ -540,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -922,6 +925,9 @@
       <c r="J22" s="9" t="s">
         <v>9</v>
       </c>
+      <c r="L22" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="6"/>
@@ -952,21 +958,21 @@
         <v>655</v>
       </c>
       <c r="F24" s="11">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="G24" s="12">
         <v>0.75</v>
       </c>
       <c r="H24" s="11">
         <f>ROUND(((F24*(1+G24)) * $B$20/$B$21)/B24, 0)</f>
-        <v>6422939</v>
+        <v>3339928</v>
       </c>
       <c r="I24" s="11">
         <v>0.81499999999999995</v>
       </c>
       <c r="J24" s="13">
         <f t="shared" ref="J24" si="5">LOG(H24*C24,2)</f>
-        <v>27.659196283614612</v>
+        <v>26.715779691033887</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15.75" thickBot="1"/>

</xml_diff>

<commit_message>
qpsk 600 limit adjust
</commit_message>
<xml_diff>
--- a/LoopIntegralReference.xlsx
+++ b/LoopIntegralReference.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninocarrillo/github/N9600A-sim/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E482C50D-12E1-854B-BA4D-82447DEC8488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11985" yWindow="45" windowWidth="16785" windowHeight="14385"/>
+    <workbookView xWindow="11980" yWindow="40" windowWidth="16780" windowHeight="14380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="21">
   <si>
     <t>BPSK 300</t>
   </si>
@@ -89,13 +95,16 @@
   </si>
   <si>
     <t>adjust for 13 hz offset</t>
+  </si>
+  <si>
+    <t>adjust limits</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,9 +266,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -297,7 +306,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -331,6 +340,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -365,9 +375,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -540,27 +551,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1">
+    <row r="1" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
@@ -574,7 +585,7 @@
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -590,7 +601,7 @@
       <c r="I2" s="4"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -606,7 +617,7 @@
       <c r="I3" s="7"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="B4" t="s">
         <v>8</v>
@@ -624,7 +635,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" t="s">
         <v>4</v>
@@ -634,7 +645,7 @@
       </c>
       <c r="J5" s="9"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" thickBot="1">
+    <row r="6" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>0</v>
       </c>
@@ -670,8 +681,8 @@
         <v>28.414244433257871</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" thickBot="1"/>
-    <row r="8" spans="1:12">
+    <row r="7" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -687,7 +698,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
@@ -703,7 +714,7 @@
       <c r="I9" s="7"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="B10" t="s">
         <v>8</v>
@@ -724,7 +735,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" t="s">
         <v>4</v>
@@ -734,7 +745,7 @@
       </c>
       <c r="J11" s="9"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" thickBot="1">
+    <row r="12" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>2</v>
       </c>
@@ -770,10 +781,10 @@
         <v>28.414244433257871</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1">
+    <row r="13" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
@@ -789,7 +800,7 @@
       <c r="I14" s="4"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>6</v>
       </c>
@@ -808,7 +819,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="B16" t="s">
         <v>8</v>
@@ -826,7 +837,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" t="s">
         <v>4</v>
@@ -836,7 +847,7 @@
       </c>
       <c r="J17" s="9"/>
     </row>
-    <row r="18" spans="1:12" ht="15.75" thickBot="1">
+    <row r="18" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>1</v>
       </c>
@@ -872,8 +883,8 @@
         <v>27.424608507342434</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" thickBot="1"/>
-    <row r="20" spans="1:12">
+    <row r="19" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>5</v>
       </c>
@@ -889,7 +900,7 @@
       <c r="I20" s="4"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>6</v>
       </c>
@@ -908,7 +919,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
       <c r="B22" t="s">
         <v>8</v>
@@ -929,7 +940,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" t="s">
         <v>4</v>
@@ -939,7 +950,7 @@
       </c>
       <c r="J23" s="9"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75" thickBot="1">
+    <row r="24" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>1</v>
       </c>
@@ -975,8 +986,8 @@
         <v>26.715779691033887</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15.75" thickBot="1"/>
-    <row r="26" spans="1:12">
+    <row r="25" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>5</v>
       </c>
@@ -992,7 +1003,7 @@
       <c r="I26" s="4"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>6</v>
       </c>
@@ -1008,7 +1019,7 @@
       <c r="I27" s="7"/>
       <c r="J27" s="8"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
       <c r="B28" t="s">
         <v>8</v>
@@ -1029,7 +1040,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" t="s">
         <v>4</v>
@@ -1042,7 +1053,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15.75" thickBot="1">
+    <row r="30" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>3</v>
       </c>
@@ -1078,8 +1089,8 @@
         <v>28.416995678270762</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="15.75" thickBot="1"/>
-    <row r="32" spans="1:12">
+    <row r="31" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>5</v>
       </c>
@@ -1095,7 +1106,7 @@
       <c r="I32" s="4"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>6</v>
       </c>
@@ -1111,7 +1122,7 @@
       <c r="I33" s="7"/>
       <c r="J33" s="8"/>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="6"/>
       <c r="B34" t="s">
         <v>8</v>
@@ -1132,7 +1143,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
       <c r="B35" t="s">
         <v>4</v>
@@ -1145,7 +1156,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15.75" thickBot="1">
+    <row r="36" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>3</v>
       </c>
@@ -1181,8 +1192,8 @@
         <v>28.416995255606221</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="15.75" thickBot="1"/>
-    <row r="38" spans="1:12">
+    <row r="37" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>5</v>
       </c>
@@ -1198,7 +1209,7 @@
       <c r="I38" s="4"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>6</v>
       </c>
@@ -1214,7 +1225,7 @@
       <c r="I39" s="7"/>
       <c r="J39" s="8"/>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="6"/>
       <c r="B40" t="s">
         <v>8</v>
@@ -1232,7 +1243,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
       <c r="B41" t="s">
         <v>4</v>
@@ -1242,7 +1253,7 @@
       </c>
       <c r="J41" s="9"/>
     </row>
-    <row r="42" spans="1:12" ht="15.75" thickBot="1">
+    <row r="42" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>0</v>
       </c>
@@ -1278,8 +1289,8 @@
         <v>28.416995255606221</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="15.75" thickBot="1"/>
-    <row r="44" spans="1:12">
+    <row r="43" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>5</v>
       </c>
@@ -1295,7 +1306,7 @@
       <c r="I44" s="4"/>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>6</v>
       </c>
@@ -1311,7 +1322,7 @@
       <c r="I45" s="7"/>
       <c r="J45" s="8"/>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="6"/>
       <c r="B46" t="s">
         <v>8</v>
@@ -1329,7 +1340,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
       <c r="B47" t="s">
         <v>4</v>
@@ -1339,7 +1350,7 @@
       </c>
       <c r="J47" s="9"/>
     </row>
-    <row r="48" spans="1:12" ht="15.75" thickBot="1">
+    <row r="48" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
         <v>2</v>
       </c>
@@ -1375,8 +1386,8 @@
         <v>28.639387375039352</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="15.75" thickBot="1"/>
-    <row r="50" spans="1:12">
+    <row r="49" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>5</v>
       </c>
@@ -1392,7 +1403,7 @@
       <c r="I50" s="4"/>
       <c r="J50" s="5"/>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>6</v>
       </c>
@@ -1408,7 +1419,7 @@
       <c r="I51" s="7"/>
       <c r="J51" s="8"/>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="6"/>
       <c r="B52" t="s">
         <v>8</v>
@@ -1429,7 +1440,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="6"/>
       <c r="B53" t="s">
         <v>4</v>
@@ -1439,7 +1450,7 @@
       </c>
       <c r="J53" s="9"/>
     </row>
-    <row r="54" spans="1:12" ht="15.75" thickBot="1">
+    <row r="54" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
         <v>3</v>
       </c>
@@ -1473,6 +1484,109 @@
       <c r="J54" s="13">
         <f t="shared" ref="J54" si="10">LOG(H54*C54,2)</f>
         <v>27.416995678270766</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" s="3">
+        <v>65536</v>
+      </c>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="5"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A57" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57">
+        <v>14400</v>
+      </c>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
+      <c r="I57" s="7"/>
+      <c r="J57" s="8"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A58" s="6"/>
+      <c r="B58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58">
+        <v>20</v>
+      </c>
+      <c r="D58" t="s">
+        <v>10</v>
+      </c>
+      <c r="E58">
+        <v>15</v>
+      </c>
+      <c r="J58" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="L58" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A59" s="6"/>
+      <c r="B59" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" t="s">
+        <v>7</v>
+      </c>
+      <c r="J59" s="9"/>
+      <c r="L59" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B60" s="14">
+        <v>3.1000000000000001E-5</v>
+      </c>
+      <c r="C60" s="11">
+        <f>ROUND(POWER(2,$C$16)*B60, 0)</f>
+        <v>33</v>
+      </c>
+      <c r="D60" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="E60" s="11">
+        <f t="shared" ref="E60" si="11">ROUND(POWER(2,$E$4)*D60, 0)</f>
+        <v>655</v>
+      </c>
+      <c r="F60" s="11">
+        <v>13</v>
+      </c>
+      <c r="G60" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="H60" s="11">
+        <f>ROUND(((F60*(1+G60)) * $B$20/$B$21)/B60, 0)</f>
+        <v>2385663</v>
+      </c>
+      <c r="I60" s="11">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="J60" s="13">
+        <f t="shared" ref="J60" si="12">LOG(H60*C60,2)</f>
+        <v>26.230352950254424</v>
       </c>
     </row>
   </sheetData>
@@ -1485,24 +1599,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update loop refernce excel
</commit_message>
<xml_diff>
--- a/LoopIntegralReference.xlsx
+++ b/LoopIntegralReference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninocarrillo/github/N9600A-sim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37F14C9-16F9-A24E-85A6-C8900096E13B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580DF894-F75F-5646-9D37-B64B79F14E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11980" yWindow="40" windowWidth="16780" windowHeight="14380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -579,7 +579,7 @@
   <dimension ref="A1:L66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
+      <selection activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1679,35 +1679,35 @@
         <v>21</v>
       </c>
       <c r="B66" s="14">
-        <v>6.0000000000000002E-5</v>
+        <v>1E-3</v>
       </c>
       <c r="C66" s="11">
         <f>ROUND(POWER(2,$C$16)*B66, 0)</f>
-        <v>63</v>
+        <v>1049</v>
       </c>
       <c r="D66" s="11">
-        <v>3.3329999999999999E-2</v>
+        <v>0.25</v>
       </c>
       <c r="E66" s="11">
         <f t="shared" ref="E66" si="13">ROUND(POWER(2,$E$4)*D66, 0)</f>
-        <v>1092</v>
+        <v>8192</v>
       </c>
       <c r="F66" s="11">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G66" s="12">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="H66" s="11">
         <f>ROUND(((F66*(1+G66)) * $B$20/$B$21)/B66, 0)</f>
-        <v>504415</v>
+        <v>68267</v>
       </c>
       <c r="I66" s="11">
         <v>0.81499999999999995</v>
       </c>
       <c r="J66" s="13">
         <f t="shared" ref="J66" si="14">LOG(H66*C66,2)</f>
-        <v>24.921531576267107</v>
+        <v>26.09369969602302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>